<commit_message>
Full model of the box. Some updated parts for the parts list.
</commit_message>
<xml_diff>
--- a/parts.xlsx
+++ b/parts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>£</t>
   </si>
@@ -73,6 +73,18 @@
   </si>
   <si>
     <t>12V socket, 2.1mm, centre-positive</t>
+  </si>
+  <si>
+    <t>CLIFF ELECTRONIC COMPONENTS - FC681473 - CONNECTOR, RECEPTACLE, DC POWER, 2.1MM</t>
+  </si>
+  <si>
+    <t>CPC</t>
+  </si>
+  <si>
+    <t>Strut Hinges For Flight Case Lids - One Pair - Nickel Finish</t>
+  </si>
+  <si>
+    <t>Clear acrylic 4mmx100mmx200mm</t>
   </si>
 </sst>
 </file>
@@ -82,7 +94,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -156,9 +168,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="3"/>
     <xf numFmtId="44" fontId="2" fillId="2" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -257,75 +269,75 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -392,18 +404,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G10" totalsRowCount="1" headerRowDxfId="8" dataDxfId="9" headerRowCellStyle="Currency" dataCellStyle="Currency">
-  <autoFilter ref="A1:G9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G12" totalsRowCount="1" headerRowDxfId="12" dataDxfId="11" headerRowCellStyle="Currency" dataCellStyle="Currency">
+  <autoFilter ref="A1:G11"/>
   <tableColumns count="7">
-    <tableColumn id="7" name="Seller" dataDxfId="7" totalsRowDxfId="4" dataCellStyle="Currency"/>
+    <tableColumn id="7" name="Seller" dataDxfId="10" totalsRowDxfId="4" dataCellStyle="Currency"/>
     <tableColumn id="1" name="Item" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Qty" dataDxfId="5" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="£ Per" dataDxfId="6" totalsRowDxfId="3" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="£" dataDxfId="12" totalsRowDxfId="2" dataCellStyle="Currency">
+    <tableColumn id="2" name="Qty" dataDxfId="9" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="£ Per" dataDxfId="8" totalsRowDxfId="3" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="£" dataDxfId="7" totalsRowDxfId="2" dataCellStyle="Currency">
       <calculatedColumnFormula>C2*D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="PP" dataDxfId="11" totalsRowDxfId="1" dataCellStyle="Currency"/>
-    <tableColumn id="6" name="Subtotal" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="0" dataCellStyle="Currency">
+    <tableColumn id="5" name="PP" dataDxfId="6" totalsRowDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="6" name="Subtotal" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="0" dataCellStyle="Currency">
       <calculatedColumnFormula>E2+F2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -674,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,14 +737,14 @@
         <v>3.69</v>
       </c>
       <c r="E2" s="9">
-        <f>C2*D2</f>
+        <f t="shared" ref="E2:E8" si="0">C2*D2</f>
         <v>14.76</v>
       </c>
       <c r="F2" s="9">
         <v>0.99</v>
       </c>
       <c r="G2" s="9">
-        <f>E2+F2</f>
+        <f t="shared" ref="G2:G8" si="1">E2+F2</f>
         <v>15.75</v>
       </c>
     </row>
@@ -750,14 +762,14 @@
         <v>0.99</v>
       </c>
       <c r="E3" s="9">
-        <f>C3*D3</f>
+        <f t="shared" si="0"/>
         <v>0.99</v>
       </c>
       <c r="F3" s="9">
         <v>0.99</v>
       </c>
       <c r="G3" s="9">
-        <f>E3+F3</f>
+        <f t="shared" si="1"/>
         <v>1.98</v>
       </c>
     </row>
@@ -775,14 +787,14 @@
         <v>6.99</v>
       </c>
       <c r="E4" s="9">
-        <f>C4*D4</f>
+        <f t="shared" si="0"/>
         <v>6.99</v>
       </c>
       <c r="F4" s="9">
         <v>0</v>
       </c>
       <c r="G4" s="9">
-        <f>E4+F4</f>
+        <f t="shared" si="1"/>
         <v>6.99</v>
       </c>
     </row>
@@ -800,12 +812,12 @@
         <v>0.99</v>
       </c>
       <c r="E5" s="9">
-        <f>C5*D5</f>
+        <f t="shared" si="0"/>
         <v>0.99</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9">
-        <f>E5+F5</f>
+        <f t="shared" si="1"/>
         <v>0.99</v>
       </c>
     </row>
@@ -821,14 +833,14 @@
         <v>0</v>
       </c>
       <c r="E6" s="4">
-        <f>C6*D6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F6" s="4">
         <v>0</v>
       </c>
       <c r="G6" s="4">
-        <f>E6+F6</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -840,12 +852,12 @@
       <c r="C7" s="11"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4">
-        <f>C7*D7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4">
-        <f>E7+F7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -863,43 +875,107 @@
         <v>1.89</v>
       </c>
       <c r="E8" s="9">
-        <f>C8*D8</f>
+        <f t="shared" si="0"/>
         <v>3.78</v>
       </c>
       <c r="F8" s="9">
         <v>0.88</v>
       </c>
       <c r="G8" s="9">
-        <f>E8+F8</f>
+        <f t="shared" si="1"/>
         <v>4.66</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="A9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="11">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.38</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" ref="E9" si="2">C9*D9</f>
+        <v>0.38</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1.88</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" ref="G9" si="3">E9+F9</f>
+        <v>2.2599999999999998</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" t="s">
+      <c r="A10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="12">
+        <v>1</v>
+      </c>
+      <c r="D10" s="9">
+        <v>4.49</v>
+      </c>
+      <c r="E10" s="9">
+        <f>C10*D10</f>
+        <v>4.49</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9">
+        <f>E10+F10</f>
+        <v>4.49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="12">
+        <v>2</v>
+      </c>
+      <c r="D11" s="9">
+        <v>3.16</v>
+      </c>
+      <c r="E11" s="9">
+        <f>C11*D11</f>
+        <v>6.32</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9">
+        <f>E11+F11</f>
+        <v>6.32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="C10"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="2">
+      <c r="C12"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="2">
         <f>SUBTOTAL(109,Table1[Subtotal])</f>
-        <v>30.369999999999997</v>
+        <v>43.44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add display driver schematic.
</commit_message>
<xml_diff>
--- a/parts.xlsx
+++ b/parts.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="BOM" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="72">
   <si>
     <t>£</t>
   </si>
@@ -115,6 +116,132 @@
   </si>
   <si>
     <t>Arduino Pro Mini</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>REF</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Pin Header</t>
+  </si>
+  <si>
+    <t>Footprint</t>
+  </si>
+  <si>
+    <t>1x12</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>PROMICRO_A</t>
+  </si>
+  <si>
+    <t>PROMICRO_B</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>Bornier2</t>
+  </si>
+  <si>
+    <t>PANEL_2</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>Connector</t>
+  </si>
+  <si>
+    <t>PANEL_1</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>Bornier3</t>
+  </si>
+  <si>
+    <t>DIAL</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>POWER</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>MOSFET</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>TO-220</t>
+  </si>
+  <si>
+    <t>LM317T</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>330R</t>
+  </si>
+  <si>
+    <t>10-pack HARWIN - M20-9820406 - 0.1" VERTICAL SOCKET 4 WAY</t>
+  </si>
+  <si>
+    <t>MULTICOMP - 2226A-08 - CRIMP HOUSING, 1 ROW, 8 WAY</t>
+  </si>
+  <si>
+    <t>MULTICOMP - 2226TG - CRIMP TERMINAL, 24-28AWG</t>
+  </si>
+  <si>
+    <t>STARCONN CONNECTORS - IDCW-26-SC - 0.1" IDC SOCKET - 26 WAY / BUMP</t>
+  </si>
+  <si>
+    <t>STARCONN CONNECTORS - BHW-26DV - 0.1" BOX HEADER - 26 WAY</t>
   </si>
 </sst>
 </file>
@@ -214,7 +341,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -236,6 +363,10 @@
     <xf numFmtId="44" fontId="5" fillId="3" borderId="0" xfId="5" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="5"/>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="5" builtinId="27"/>
@@ -682,8 +813,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:G17" totalsRowCount="1" headerRowDxfId="25" dataDxfId="24" headerRowCellStyle="Currency" dataCellStyle="Currency">
-  <autoFilter ref="A3:G16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:G22" totalsRowCount="1" headerRowDxfId="25" dataDxfId="24" headerRowCellStyle="Currency" dataCellStyle="Currency">
+  <autoFilter ref="A3:G21"/>
   <tableColumns count="7">
     <tableColumn id="7" name="Seller" dataDxfId="23" totalsRowDxfId="4" dataCellStyle="Currency"/>
     <tableColumn id="1" name="Item" totalsRowLabel="Total"/>
@@ -718,6 +849,19 @@
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:D14" totalsRowShown="0">
+  <autoFilter ref="A1:D14"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="REF"/>
+    <tableColumn id="2" name="Type"/>
+    <tableColumn id="3" name="Footprint"/>
+    <tableColumn id="4" name="Value"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -987,7 +1131,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,12 +1371,12 @@
         <v>4.49</v>
       </c>
       <c r="E11" s="9">
-        <f>C11*D11</f>
+        <f t="shared" ref="E11:E16" si="4">C11*D11</f>
         <v>4.49</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9">
-        <f>E11+F11</f>
+        <f t="shared" ref="G11:G16" si="5">E11+F11</f>
         <v>4.49</v>
       </c>
     </row>
@@ -1250,12 +1394,12 @@
         <v>3.16</v>
       </c>
       <c r="E12" s="9">
-        <f>C12*D12</f>
+        <f t="shared" si="4"/>
         <v>6.32</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9">
-        <f>E12+F12</f>
+        <f t="shared" si="5"/>
         <v>6.32</v>
       </c>
     </row>
@@ -1273,12 +1417,12 @@
         <v>1.99</v>
       </c>
       <c r="E13" s="9">
-        <f>C13*D13</f>
+        <f t="shared" si="4"/>
         <v>1.99</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9">
-        <f>E13+F13</f>
+        <f t="shared" si="5"/>
         <v>1.99</v>
       </c>
     </row>
@@ -1296,12 +1440,12 @@
         <v>0.39</v>
       </c>
       <c r="E14" s="14">
-        <f>C14*D14</f>
+        <f t="shared" si="4"/>
         <v>0.39</v>
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="14">
-        <f>E14+F14</f>
+        <f t="shared" si="5"/>
         <v>0.39</v>
       </c>
     </row>
@@ -1319,12 +1463,12 @@
         <v>1.23</v>
       </c>
       <c r="E15" s="14">
-        <f>C15*D15</f>
+        <f t="shared" si="4"/>
         <v>1.23</v>
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="14">
-        <f>E15+F15</f>
+        <f t="shared" si="5"/>
         <v>1.23</v>
       </c>
     </row>
@@ -1342,68 +1486,139 @@
         <v>0.77</v>
       </c>
       <c r="E16" s="14">
-        <f>C16*D16</f>
+        <f t="shared" si="4"/>
         <v>0.77</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="14">
-        <f>E16+F16</f>
+        <f t="shared" si="5"/>
         <v>0.77</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="11">
+        <v>1</v>
+      </c>
+      <c r="D17" s="4">
+        <v>4.79</v>
+      </c>
+      <c r="E17" s="4">
+        <f>C17*D17</f>
+        <v>4.79</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4">
+        <f>E17+F17</f>
+        <v>4.79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="11">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="E18" s="1">
+        <f>C18*D18</f>
+        <v>0.04</v>
+      </c>
+      <c r="G18" s="1">
+        <f>E18+F18</f>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="11">
+        <v>100</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E19" s="1">
+        <f>C19*D19</f>
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
+        <f>E19+F19</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="11">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="E20" s="1">
+        <f>C20*D20</f>
+        <v>0.68</v>
+      </c>
+      <c r="G20" s="1">
+        <f>E20+F20</f>
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="11">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E21" s="1">
+        <f>C21*D21</f>
+        <v>0.5</v>
+      </c>
+      <c r="G21" s="1">
+        <f>E21+F21</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" t="s">
         <v>6</v>
       </c>
-      <c r="C17"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="2">
+      <c r="C22"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="20">
         <f>SUBTOTAL(109,Table1[Subtotal])</f>
-        <v>47.940000000000005</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="C18"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="C19"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="C20"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="C21"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="C22"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="2"/>
+        <v>54.95</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
@@ -1600,4 +1815,224 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Trying out a PCB-based LED panel instead of Veroboard.
</commit_message>
<xml_diff>
--- a/parts.xlsx
+++ b/parts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Documents\Dev\uv-box\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\uv-box\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
   <si>
     <t>£</t>
   </si>
@@ -238,10 +238,13 @@
     <t>MULTICOMP - 2226TG - CRIMP TERMINAL, 24-28AWG</t>
   </si>
   <si>
-    <t>STARCONN CONNECTORS - IDCW-26-SC - 0.1" IDC SOCKET - 26 WAY / BUMP</t>
-  </si>
-  <si>
-    <t>STARCONN CONNECTORS - BHW-26DV - 0.1" BOX HEADER - 26 WAY</t>
+    <t>5x IDC Cable Mounting Socket Connector </t>
+  </si>
+  <si>
+    <t>5x Straight IDC PCB Box Header Connector</t>
+  </si>
+  <si>
+    <t>10x Ceramic Disc Capacitors 50V 47 values</t>
   </si>
 </sst>
 </file>
@@ -813,8 +816,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:G22" totalsRowCount="1" headerRowDxfId="25" dataDxfId="24" headerRowCellStyle="Currency" dataCellStyle="Currency">
-  <autoFilter ref="A3:G21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:G23" totalsRowCount="1" headerRowDxfId="25" dataDxfId="24" headerRowCellStyle="Currency" dataCellStyle="Currency">
+  <autoFilter ref="A3:G22"/>
   <tableColumns count="7">
     <tableColumn id="7" name="Seller" dataDxfId="23" totalsRowDxfId="4" dataCellStyle="Currency"/>
     <tableColumn id="1" name="Item" totalsRowLabel="Total"/>
@@ -833,19 +836,19 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A28:G34" totalsRowCount="1" headerRowDxfId="17" dataDxfId="16" headerRowCellStyle="Currency" dataCellStyle="Currency">
-  <autoFilter ref="A28:G33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A27:G33" totalsRowCount="1" headerRowDxfId="17" dataDxfId="16" headerRowCellStyle="Currency" dataCellStyle="Currency">
+  <autoFilter ref="A27:G32"/>
   <tableColumns count="7">
     <tableColumn id="7" name="Seller" dataDxfId="15" totalsRowDxfId="14" dataCellStyle="Currency"/>
     <tableColumn id="1" name="Item" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Qty" dataDxfId="13" dataCellStyle="Comma"/>
     <tableColumn id="3" name="£ Per" dataDxfId="12" totalsRowDxfId="11" dataCellStyle="Currency"/>
     <tableColumn id="4" name="£" dataDxfId="10" totalsRowDxfId="9" dataCellStyle="Currency">
-      <calculatedColumnFormula>C29*D29</calculatedColumnFormula>
+      <calculatedColumnFormula>C28*D28</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="PP" dataDxfId="8" totalsRowDxfId="7" dataCellStyle="Currency"/>
     <tableColumn id="6" name="Subtotal" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="5" dataCellStyle="Currency">
-      <calculatedColumnFormula>E29+F29</calculatedColumnFormula>
+      <calculatedColumnFormula>E28+F28</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1128,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1563,70 +1566,91 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="A20" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="12">
+        <v>1</v>
+      </c>
+      <c r="D20" s="9">
+        <v>1</v>
+      </c>
+      <c r="E20" s="9">
+        <f>C20*D20</f>
+        <v>1</v>
+      </c>
+      <c r="F20" s="9">
+        <v>1</v>
+      </c>
+      <c r="G20" s="9">
+        <f>E20+F20</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C21" s="12">
         <v>2</v>
       </c>
-      <c r="D20" s="1">
-        <v>0.34</v>
-      </c>
-      <c r="E20" s="1">
-        <f>C20*D20</f>
-        <v>0.68</v>
-      </c>
-      <c r="G20" s="1">
-        <f>E20+F20</f>
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="11">
-        <v>2</v>
-      </c>
-      <c r="D21" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="E21" s="1">
+      <c r="D21" s="9">
+        <v>1.4</v>
+      </c>
+      <c r="E21" s="9">
         <f>C21*D21</f>
-        <v>0.5</v>
-      </c>
-      <c r="G21" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="F21" s="9">
+        <v>1</v>
+      </c>
+      <c r="G21" s="9">
         <f>E21+F21</f>
-        <v>0.5</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" t="s">
+      <c r="A22" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="12">
+        <v>1</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0.99</v>
+      </c>
+      <c r="E22" s="9">
+        <f>C22*D22</f>
+        <v>0.99</v>
+      </c>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9">
+        <f>E22+F22</f>
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="18"/>
+      <c r="B23" t="s">
         <v>6</v>
       </c>
-      <c r="C22"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="20">
+      <c r="C23"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="20">
         <f>SUBTOTAL(109,Table1[Subtotal])</f>
-        <v>54.95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="C23"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="2"/>
+        <v>60.56</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
@@ -1636,173 +1660,165 @@
       <c r="F24" s="3"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="C25"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="13" t="s">
+    <row r="25" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C27"/>
-      <c r="D27"/>
-      <c r="E27"/>
-      <c r="F27"/>
+    <row r="26" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>5</v>
+      <c r="A28" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="12">
+        <v>1</v>
+      </c>
+      <c r="D28" s="9">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="E28" s="9">
+        <f>C28*D28</f>
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9">
+        <f>E28+F28</f>
+        <v>8.9499999999999993</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C29" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" s="9">
-        <v>8.9499999999999993</v>
+        <v>3.7</v>
       </c>
       <c r="E29" s="9">
         <f>C29*D29</f>
-        <v>8.9499999999999993</v>
+        <v>7.4</v>
       </c>
       <c r="F29" s="9"/>
-      <c r="G29" s="9">
+      <c r="G29" s="4">
         <f>E29+F29</f>
-        <v>8.9499999999999993</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B30" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="11">
+      <c r="B30" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="12">
         <v>2</v>
       </c>
-      <c r="D30" s="4">
-        <v>3.7</v>
-      </c>
-      <c r="E30" s="4">
+      <c r="D30" s="9">
+        <v>3.89</v>
+      </c>
+      <c r="E30" s="9">
         <f>C30*D30</f>
-        <v>7.4</v>
-      </c>
-      <c r="F30" s="4"/>
+        <v>7.78</v>
+      </c>
+      <c r="F30" s="9"/>
       <c r="G30" s="4">
         <f>E30+F30</f>
-        <v>7.4</v>
+        <v>7.78</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B31" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" s="11">
-        <v>2</v>
-      </c>
-      <c r="D31" s="4">
-        <v>3.89</v>
-      </c>
-      <c r="E31" s="4">
+      <c r="B31" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="12">
+        <v>1</v>
+      </c>
+      <c r="D31" s="9">
+        <v>4.04</v>
+      </c>
+      <c r="E31" s="9">
         <f>C31*D31</f>
-        <v>7.78</v>
-      </c>
-      <c r="F31" s="4"/>
+        <v>4.04</v>
+      </c>
+      <c r="F31" s="9"/>
       <c r="G31" s="4">
         <f>E31+F31</f>
-        <v>7.78</v>
+        <v>4.04</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B32" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" s="11">
-        <v>1</v>
-      </c>
-      <c r="D32" s="4">
-        <v>4.04</v>
-      </c>
-      <c r="E32" s="4">
+      <c r="B32" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="12">
+        <v>1</v>
+      </c>
+      <c r="D32" s="9">
+        <v>5.62</v>
+      </c>
+      <c r="E32" s="9">
         <f>C32*D32</f>
-        <v>4.04</v>
-      </c>
-      <c r="F32" s="4"/>
+        <v>5.62</v>
+      </c>
+      <c r="F32" s="9"/>
       <c r="G32" s="4">
         <f>E32+F32</f>
-        <v>4.04</v>
+        <v>5.62</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="A33" s="5"/>
       <c r="B33" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="11">
-        <v>1</v>
-      </c>
-      <c r="D33" s="4">
-        <v>5.62</v>
-      </c>
-      <c r="E33" s="4">
-        <f>C33*D33</f>
-        <v>5.62</v>
-      </c>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4">
-        <f>E33+F33</f>
-        <v>5.62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" t="s">
         <v>6</v>
       </c>
-      <c r="C34"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="2">
+      <c r="C33"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="2">
         <f>SUBTOTAL(109,Table13[Subtotal])</f>
         <v>33.79</v>
       </c>

</xml_diff>